<commit_message>
re-doing all plots and tables
</commit_message>
<xml_diff>
--- a/3 TP Analysis/04 - Tables/Cover_averaged_over_3TP.xlsx
+++ b/3 TP Analysis/04 - Tables/Cover_averaged_over_3TP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shannon/GitHub/NFI_benthic_community/3 TP Analysis/04 - Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B468861F-A3F3-AF48-ADE0-8381ECE0D68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F428D6F0-1372-2740-BECD-46B64F26BC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="500" windowWidth="26360" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="25880" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -66,10 +66,10 @@
     <t>Turf</t>
   </si>
   <si>
+    <t>Benthic category</t>
+  </si>
+  <si>
     <t>Cover (%)</t>
-  </si>
-  <si>
-    <t>Benthic category</t>
   </si>
   <si>
     <t>Slaughter Bay</t>
@@ -114,9 +114,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -413,392 +412,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="208" workbookViewId="0">
       <selection sqref="A1:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
-        <v>3.94</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0.2</v>
       </c>
-      <c r="D3" s="1">
-        <v>3.94</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>13.25</v>
       </c>
-      <c r="D4" s="1">
-        <v>3.94</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>24.98</v>
       </c>
-      <c r="D5" s="1">
-        <v>3.94</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>0.84</v>
       </c>
-      <c r="D6" s="1">
-        <v>3.94</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
-        <v>23.64</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3.94</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>23.65</v>
+      </c>
+      <c r="D7">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.54</v>
       </c>
-      <c r="D8" s="1">
-        <v>3.94</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>28.24</v>
       </c>
-      <c r="D9" s="1">
-        <v>3.94</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D10" s="1">
-        <v>3.94</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D12" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>17.190000000000001</v>
       </c>
-      <c r="D13" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>30.12</v>
       </c>
-      <c r="D14" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.79</v>
       </c>
-      <c r="D15" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>16.12</v>
       </c>
-      <c r="D16" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0.7</v>
       </c>
-      <c r="D17" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>29.82</v>
       </c>
-      <c r="D18" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>5.12</v>
       </c>
-      <c r="D19" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>0</v>
       </c>
-      <c r="D20" s="1">
-        <v>4.71</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>1.69</v>
       </c>
-      <c r="D21" s="1">
-        <v>4.71</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>7.76</v>
       </c>
-      <c r="D22" s="1">
-        <v>4.71</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>37.47</v>
       </c>
-      <c r="D23" s="1">
-        <v>4.71</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>0.86</v>
       </c>
-      <c r="D24" s="1">
-        <v>4.71</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>12.15</v>
       </c>
-      <c r="D25" s="1">
-        <v>4.71</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>0.63</v>
       </c>
-      <c r="D26" s="1">
-        <v>4.71</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>32.29</v>
       </c>
-      <c r="D27" s="1">
-        <v>4.71</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>7.13</v>
       </c>
-      <c r="D28" s="1">
-        <v>4.71</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="D28">
+        <v>4.71</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>